<commit_message>
Darkwulf1986 X5SA Repo V1.21
</commit_message>
<xml_diff>
--- a/Rotational Distance xlsx/Rotation Distance.xlsx
+++ b/Rotational Distance xlsx/Rotation Distance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Rotation Distance from Printer.cfg</t>
   </si>
@@ -271,11 +271,53 @@
   <si>
     <t>3. Write down measured values as &lt;Actual Print Distance&gt;.</t>
   </si>
+  <si>
+    <t>Düsendurchmesser:</t>
+  </si>
+  <si>
+    <t>Layer height:</t>
+  </si>
+  <si>
+    <t>Nozzle diameter:</t>
+  </si>
+  <si>
+    <t>Speed for 1 second in mm:</t>
+  </si>
+  <si>
+    <t>Geschwindigkeit für 1 Sekunde in mm:</t>
+  </si>
+  <si>
+    <t>Schichthöhe:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,75mm Filament: </t>
+  </si>
+  <si>
+    <t>2,41 mm²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,85mm Filament: </t>
+  </si>
+  <si>
+    <t>6,38 mm²</t>
+  </si>
+  <si>
+    <t>Flächeninhalt Filament:</t>
+  </si>
+  <si>
+    <t>Flowrate Calculator:</t>
+  </si>
+  <si>
+    <t>Filament area:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00\ &quot;mm³&quot;"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -346,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,8 +455,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -568,29 +628,185 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="13" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,29 +815,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -916,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U52"/>
+  <dimension ref="A1:U63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -931,70 +1126,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24" thickBot="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:21" s="17" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:21" s="8" customFormat="1" ht="36.75" customHeight="1">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="1:21" s="5" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A3" s="6">
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="1:21" s="2" customFormat="1" ht="34.5" customHeight="1">
+      <c r="A3" s="3">
         <v>33</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="4">
         <v>29</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="36">
         <v>30</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="37"/>
     </row>
     <row r="4" spans="1:21" ht="21">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="39"/>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1" thickBot="1">
-      <c r="A5" s="8">
+      <c r="A5" s="5">
         <f>(A3*B3)/C3</f>
         <v>31.9</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="18.75">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="41"/>
+      <c r="C9" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
     </row>
     <row r="10" spans="1:21" ht="18.75">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1004,31 +1199,31 @@
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="18"/>
+      <c r="A12" s="9"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.75">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15.75">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15.75">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="9" t="s">
         <v>10</v>
       </c>
       <c r="U16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="15.75">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1038,28 +1233,28 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="18.75">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="20" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
     </row>
     <row r="22" spans="1:10" ht="18.75">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1069,17 +1264,17 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1094,7 +1289,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="18.75">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1137,7 +1332,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="11" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1156,12 +1351,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -1169,19 +1364,98 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:10">
       <c r="B51" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:10">
       <c r="B52" t="s">
         <v>38</v>
       </c>
     </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="59" spans="1:10">
+      <c r="A59" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G59" s="23"/>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A60" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F60" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G60" s="27"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="18">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B61" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C61" s="18">
+        <v>30</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G61" s="24"/>
+      <c r="H61" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A62" s="15"/>
+      <c r="F62" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G62" s="25"/>
+      <c r="H62" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15.75" thickTop="1">
+      <c r="A63" s="21">
+        <f>A61*B61*C61</f>
+        <v>2.3100000000000005</v>
+      </c>
+      <c r="B63" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D21:J21"/>
+  <mergeCells count="12">
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
@@ -1189,6 +1463,11 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="D21:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Darkwulf1986 X5SA Repo V1.23
</commit_message>
<xml_diff>
--- a/Rotational Distance xlsx/Rotation Distance.xlsx
+++ b/Rotational Distance xlsx/Rotation Distance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Rotation Distance from Printer.cfg</t>
   </si>
@@ -310,13 +310,38 @@
   <si>
     <t>Filament area:</t>
   </si>
+  <si>
+    <t>(Spiralisierter Würfel)</t>
+  </si>
+  <si>
+    <t>(Spiralised cube)</t>
+  </si>
+  <si>
+    <t>Flowrate Rechner für hohlen Testwürfel:</t>
+  </si>
+  <si>
+    <t>Flowrate Calculator for Hollow Test Cube:</t>
+  </si>
+  <si>
+    <t>Erster Druck Überschuss zum gewünschten Ergebnis !!!</t>
+  </si>
+  <si>
+    <t>First print surplus to the desired result !!!!</t>
+  </si>
+  <si>
+    <t>Result must always be calculated to 100 %.</t>
+  </si>
+  <si>
+    <t>Ergebnis muss immer auf 100 % berechnet werden.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;mm³&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.00\ &quot;%&quot;"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -388,7 +413,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,8 +498,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -732,11 +769,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -781,6 +891,8 @@
     <xf numFmtId="164" fontId="1" fillId="13" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -817,12 +929,28 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1111,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U63"/>
+  <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1126,12 +1254,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24" thickBot="1">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="36.75" customHeight="1">
       <c r="A2" s="7" t="s">
@@ -1140,10 +1268,10 @@
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="35"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="34.5" customHeight="1">
       <c r="A3" s="3">
@@ -1152,10 +1280,10 @@
       <c r="B3" s="4">
         <v>29</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="38">
         <v>30</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="39"/>
     </row>
     <row r="4" spans="1:21" ht="21">
       <c r="A4" s="6" t="s">
@@ -1164,10 +1292,10 @@
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="41"/>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1" thickBot="1">
       <c r="A5" s="5">
@@ -1176,17 +1304,17 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="18.75">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="28" t="s">
+      <c r="B9" s="43"/>
+      <c r="C9" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:21" ht="18.75">
       <c r="A10" s="11" t="s">
@@ -1233,20 +1361,20 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="18.75">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="28" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
     </row>
     <row r="22" spans="1:10" ht="18.75">
       <c r="A22" s="12" t="s">
@@ -1399,10 +1527,10 @@
       <c r="C59" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F59" s="22" t="s">
+      <c r="F59" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G59" s="23"/>
+      <c r="G59" s="25"/>
     </row>
     <row r="60" spans="1:10" ht="15.75" thickBot="1">
       <c r="A60" s="20" t="s">
@@ -1414,10 +1542,10 @@
       <c r="C60" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F60" s="26" t="s">
+      <c r="F60" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="G60" s="27"/>
+      <c r="G60" s="29"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="18">
@@ -1429,20 +1557,20 @@
       <c r="C61" s="18">
         <v>30</v>
       </c>
-      <c r="F61" s="24" t="s">
+      <c r="F61" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="G61" s="24"/>
+      <c r="G61" s="26"/>
       <c r="H61" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15.75" thickBot="1">
       <c r="A62" s="15"/>
-      <c r="F62" s="25" t="s">
+      <c r="F62" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="G62" s="25"/>
+      <c r="G62" s="27"/>
       <c r="H62" s="17" t="s">
         <v>50</v>
       </c>
@@ -1454,8 +1582,69 @@
       </c>
       <c r="B63" s="14"/>
     </row>
+    <row r="66" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="67" spans="1:3">
+      <c r="A67" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A68" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A69" s="44">
+        <v>0.25</v>
+      </c>
+      <c r="B69" s="45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A70" s="22"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="23">
+        <f>A69*100/B69</f>
+        <v>50</v>
+      </c>
+      <c r="B71" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" s="49"/>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B72" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="C72" s="51"/>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="74" spans="1:3">
+      <c r="B74" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" s="53"/>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" thickBot="1">
+      <c r="B75" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C75" s="51"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>

</xml_diff>

<commit_message>
Darkwulf1986 X5SA Repo V1.24
</commit_message>
<xml_diff>
--- a/Rotational Distance xlsx/Rotation Distance.xlsx
+++ b/Rotational Distance xlsx/Rotation Distance.xlsx
@@ -893,42 +893,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
@@ -940,6 +904,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1242,7 +1242,7 @@
   <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1254,12 +1254,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24" thickBot="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="36.75" customHeight="1">
       <c r="A2" s="7" t="s">
@@ -1268,10 +1268,10 @@
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="41"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="34.5" customHeight="1">
       <c r="A3" s="3">
@@ -1280,10 +1280,10 @@
       <c r="B3" s="4">
         <v>29</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="42">
         <v>30</v>
       </c>
-      <c r="D3" s="39"/>
+      <c r="D3" s="43"/>
     </row>
     <row r="4" spans="1:21" ht="21">
       <c r="A4" s="6" t="s">
@@ -1292,10 +1292,10 @@
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="45"/>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1" thickBot="1">
       <c r="A5" s="5">
@@ -1304,17 +1304,17 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="18.75">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="30" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
     </row>
     <row r="10" spans="1:21" ht="18.75">
       <c r="A10" s="11" t="s">
@@ -1361,20 +1361,20 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="18.75">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="30" t="s">
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
     </row>
     <row r="22" spans="1:10" ht="18.75">
       <c r="A22" s="12" t="s">
@@ -1527,10 +1527,10 @@
       <c r="C59" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F59" s="24" t="s">
+      <c r="F59" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="G59" s="25"/>
+      <c r="G59" s="50"/>
     </row>
     <row r="60" spans="1:10" ht="15.75" thickBot="1">
       <c r="A60" s="20" t="s">
@@ -1542,35 +1542,35 @@
       <c r="C60" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F60" s="28" t="s">
+      <c r="F60" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="G60" s="29"/>
+      <c r="G60" s="54"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="18">
-        <v>0.55000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="B61" s="18">
         <v>0.14000000000000001</v>
       </c>
       <c r="C61" s="18">
-        <v>30</v>
-      </c>
-      <c r="F61" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F61" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="G61" s="26"/>
+      <c r="G61" s="51"/>
       <c r="H61" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15.75" thickBot="1">
       <c r="A62" s="15"/>
-      <c r="F62" s="27" t="s">
+      <c r="F62" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="G62" s="27"/>
+      <c r="G62" s="52"/>
       <c r="H62" s="17" t="s">
         <v>50</v>
       </c>
@@ -1578,33 +1578,33 @@
     <row r="63" spans="1:10" ht="15.75" thickTop="1">
       <c r="A63" s="21">
         <f>A61*B61*C61</f>
-        <v>2.3100000000000005</v>
+        <v>6.7200000000000006</v>
       </c>
       <c r="B63" s="14"/>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="67" spans="1:3">
-      <c r="A67" s="46" t="s">
+      <c r="A67" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B67" s="46" t="s">
+      <c r="B67" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A68" s="47" t="s">
+      <c r="A68" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B68" s="47" t="s">
+      <c r="B68" s="27" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A69" s="44">
-        <v>0.25</v>
-      </c>
-      <c r="B69" s="45">
-        <v>0.5</v>
+      <c r="A69" s="24">
+        <v>0.64</v>
+      </c>
+      <c r="B69" s="25">
+        <v>0.6</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
@@ -1613,50 +1613,50 @@
     <row r="71" spans="1:3">
       <c r="A71" s="23">
         <f>A69*100/B69</f>
-        <v>50</v>
-      </c>
-      <c r="B71" s="48" t="s">
+        <v>106.66666666666667</v>
+      </c>
+      <c r="B71" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C71" s="49"/>
+      <c r="C71" s="29"/>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B72" s="50" t="s">
+      <c r="B72" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C72" s="51"/>
+      <c r="C72" s="31"/>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1"/>
     <row r="74" spans="1:3">
-      <c r="B74" s="52" t="s">
+      <c r="B74" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C74" s="53"/>
+      <c r="C74" s="33"/>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B75" s="54" t="s">
+      <c r="B75" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C75" s="51"/>
+      <c r="C75" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="D21:J21"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Darkwulf3D X5SA Repo V1.26
</commit_message>
<xml_diff>
--- a/Rotational Distance xlsx/Rotation Distance.xlsx
+++ b/Rotational Distance xlsx/Rotation Distance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Rotation Distance from Printer.cfg</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Wenn der tatsächliche_Extrudierabstand von dem gewünschten_Extrudierabstand um mehr als 2 mm abweicht, ist es ratsam, die obigen Schritte ein zweites Mal durchzuführen.</t>
   </si>
   <si>
-    <t>German:</t>
-  </si>
-  <si>
     <t>Section from the Klipper homepage for setting the extrusion distance</t>
   </si>
   <si>
@@ -334,14 +331,40 @@
   <si>
     <t>Ergebnis muss immer auf 100 % berechnet werden.</t>
   </si>
+  <si>
+    <t>Max Flowrate Test (Hotend)</t>
+  </si>
+  <si>
+    <t>Max. Extruder Geschwindigkeit: mm/s</t>
+  </si>
+  <si>
+    <t>Filament Durchmesser: mm</t>
+  </si>
+  <si>
+    <t>Filament Diameter: mm</t>
+  </si>
+  <si>
+    <t>Feedrate für Test Befehl: G1 E100 F..</t>
+  </si>
+  <si>
+    <t>Feedrate for Test: G1 E100 F..</t>
+  </si>
+  <si>
+    <t>Deutsch:</t>
+  </si>
+  <si>
+    <t>Max. Extrude Speed: mm/s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;mm³&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00\ &quot;%&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.00\ &quot;mm³/s&quot;"/>
+    <numFmt numFmtId="167" formatCode="&quot;F&quot;0"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -413,7 +436,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,8 +533,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -842,11 +889,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -897,6 +987,14 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="18" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -906,6 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -923,9 +1022,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -948,6 +1048,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99FF"/>
       <color rgb="FFFFFFCC"/>
     </mruColors>
   </colors>
@@ -1239,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U75"/>
+  <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1254,12 +1355,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24" thickBot="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:21" s="8" customFormat="1" ht="36.75" customHeight="1">
       <c r="A2" s="7" t="s">
@@ -1268,10 +1369,10 @@
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="41"/>
+      <c r="D2" s="50"/>
     </row>
     <row r="3" spans="1:21" s="2" customFormat="1" ht="34.5" customHeight="1">
       <c r="A3" s="3">
@@ -1280,10 +1381,10 @@
       <c r="B3" s="4">
         <v>29</v>
       </c>
-      <c r="C3" s="42">
+      <c r="C3" s="51">
         <v>30</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="52"/>
     </row>
     <row r="4" spans="1:21" ht="21">
       <c r="A4" s="6" t="s">
@@ -1292,10 +1393,10 @@
       <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1" thickBot="1">
       <c r="A5" s="5">
@@ -1304,21 +1405,21 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="18.75">
-      <c r="A9" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
+      <c r="A9" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="56"/>
+      <c r="C9" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
     </row>
     <row r="10" spans="1:21" ht="18.75">
       <c r="A10" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1352,7 +1453,7 @@
     </row>
     <row r="17" spans="1:10" ht="15.75">
       <c r="A17" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1361,24 +1462,24 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="18.75">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
     </row>
     <row r="22" spans="1:10" ht="18.75">
       <c r="A22" s="12" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1408,7 +1509,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1418,93 +1519,93 @@
     </row>
     <row r="34" spans="1:2" ht="18.75">
       <c r="A34" s="12" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="B40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="B41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75">
       <c r="A45" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" t="s">
         <v>35</v>
-      </c>
-      <c r="B50" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="B51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="B52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -1519,87 +1620,87 @@
     <row r="58" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="59" spans="1:10">
       <c r="A59" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="F59" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="G59" s="50"/>
+        <v>44</v>
+      </c>
+      <c r="F59" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="G59" s="60"/>
     </row>
     <row r="60" spans="1:10" ht="15.75" thickBot="1">
       <c r="A60" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C60" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F60" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="G60" s="54"/>
+      <c r="F60" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="G60" s="64"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="18">
         <v>0.6</v>
       </c>
       <c r="B61" s="18">
-        <v>0.14000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="C61" s="18">
-        <v>80</v>
-      </c>
-      <c r="F61" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F61" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="G61" s="61"/>
+      <c r="H61" s="16" t="s">
         <v>47</v>
-      </c>
-      <c r="G61" s="51"/>
-      <c r="H61" s="16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15.75" thickBot="1">
       <c r="A62" s="15"/>
-      <c r="F62" s="52" t="s">
+      <c r="F62" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="G62" s="62"/>
+      <c r="H62" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="G62" s="52"/>
-      <c r="H62" s="17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15.75" thickTop="1">
       <c r="A63" s="21">
         <f>A61*B61*C61</f>
-        <v>6.7200000000000006</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="B63" s="14"/>
     </row>
-    <row r="66" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="67" spans="1:3">
+    <row r="66" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="67" spans="1:10">
       <c r="A67" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A68" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B67" s="26" t="s">
+      <c r="B68" s="27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A68" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B68" s="27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" thickBot="1">
+    <row r="69" spans="1:10" ht="15.75" thickBot="1">
       <c r="A69" s="24">
         <v>0.64</v>
       </c>
@@ -1607,40 +1708,107 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
+    <row r="70" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A70" s="22"/>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:10">
       <c r="A71" s="23">
         <f>A69*100/B69</f>
         <v>106.66666666666667</v>
       </c>
-      <c r="B71" s="28" t="s">
+      <c r="B71" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71" s="37"/>
+    </row>
+    <row r="72" spans="1:10" ht="15.75" thickBot="1">
+      <c r="B72" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C71" s="29"/>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B72" s="30" t="s">
+      <c r="C72" s="39"/>
+    </row>
+    <row r="73" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="74" spans="1:10">
+      <c r="B74" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C74" s="41"/>
+    </row>
+    <row r="75" spans="1:10" ht="15.75" thickBot="1">
+      <c r="B75" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C72" s="31"/>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="74" spans="1:3">
-      <c r="B74" s="32" t="s">
+      <c r="C75" s="39"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C74" s="33"/>
-    </row>
-    <row r="75" spans="1:3" ht="15.75" thickBot="1">
-      <c r="B75" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C75" s="31"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
+      <c r="J78" s="29"/>
+    </row>
+    <row r="79" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="80" spans="1:10">
+      <c r="A80" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A81" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B81" s="33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="34">
+        <v>6</v>
+      </c>
+      <c r="B82" s="34">
+        <v>1.75</v>
+      </c>
+      <c r="E82" s="14"/>
+    </row>
+    <row r="83" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A83" s="15"/>
+    </row>
+    <row r="84" spans="1:6" ht="15.75" thickTop="1">
+      <c r="A84" s="35">
+        <f>A82*PI()*(B82/2*B82/2)</f>
+        <v>14.431691252428113</v>
+      </c>
+      <c r="C84" s="28">
+        <f>60*A82</f>
+        <v>360</v>
+      </c>
+      <c r="D84" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="E84" s="57"/>
+      <c r="F84" s="41"/>
+    </row>
+    <row r="85" spans="1:6" ht="15.75" thickBot="1">
+      <c r="D85" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E85" s="58"/>
+      <c r="F85" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="18">
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D85:F85"/>
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="F61:G61"/>
     <mergeCell ref="F62:G62"/>

</xml_diff>